<commit_message>
Datenblatt: Teileigentumseinheit-Projekt Zuordnung und Filtern by Projekt beim Hinzufügen
</commit_message>
<xml_diff>
--- a/basic/web/file/te-liste.xlsx
+++ b/basic/web/file/te-liste.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erdal\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>TE-Nummer</t>
   </si>
@@ -56,12 +52,15 @@
   </si>
   <si>
     <t>OG</t>
+  </si>
+  <si>
+    <t>Test OG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,7 +90,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -112,6 +111,17 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -135,10 +145,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -445,7 +453,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -453,15 +461,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,11 +495,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1111</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
       <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
@@ -504,16 +514,20 @@
       <c r="F2" s="6">
         <v>257000</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="5">
+        <v>4471.1203897007654</v>
+      </c>
       <c r="H2" s="5">
         <v>7.59</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2222</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
       <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
@@ -523,15 +537,84 @@
       <c r="E3" s="5">
         <v>32</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>85000</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="5">
+        <v>2656.25</v>
+      </c>
       <c r="H3" s="5">
         <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>2223</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>460000</v>
+      </c>
+      <c r="G4" s="5">
+        <v>4600</v>
+      </c>
+      <c r="H4" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>2224</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>200</v>
+      </c>
+      <c r="F5">
+        <v>920000</v>
+      </c>
+      <c r="G5" s="5">
+        <v>4600</v>
+      </c>
+      <c r="H5" s="8">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>